<commit_message>
highlighted most of what we've completed so far.
</commit_message>
<xml_diff>
--- a/documents/2016fallPracticumDeliverables.xlsx
+++ b/documents/2016fallPracticumDeliverables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\dssVisualizer\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="DSSProject_Needs" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>plugin API (import, export, open, select, modify, annotate, save, close, etc.)</t>
   </si>
   <si>
-    <t>plugin API (display, filter, search, annotate, select, modify, etc.)</t>
-  </si>
-  <si>
     <t>documentation</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>cross-platform install package</t>
   </si>
   <si>
-    <t>instantiates/executes plugins (data source and rendering plugins)</t>
-  </si>
-  <si>
     <t>pcap data protocol display plugin</t>
   </si>
   <si>
@@ -98,12 +92,73 @@
   <si>
     <t>PHASE I: List of Needs (prioritized in decreasing order)</t>
   </si>
+  <si>
+    <r>
+      <t>plugin API (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">, filter, search, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>annotate, select, modify</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>instantiates/executes plugins (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>data source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and rendering plugins)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -129,6 +184,23 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -254,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -268,7 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -280,6 +351,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +640,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -578,10 +655,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
-        <v>24</v>
+      <c r="A1" s="16" t="s">
+        <v>22</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
@@ -589,7 +666,7 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -599,38 +676,38 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="8" t="s">
-        <v>15</v>
+      <c r="A5" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
+      <c r="A6" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="9"/>
       <c r="F6" s="1"/>
@@ -643,7 +720,7 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="10"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -674,7 +751,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -687,11 +764,11 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>8</v>
+      <c r="B13" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -700,11 +777,11 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -714,10 +791,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -726,9 +803,9 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="14"/>
-      <c r="B16" s="8" t="s">
-        <v>21</v>
+      <c r="A16" s="13"/>
+      <c r="B16" s="21" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -737,9 +814,9 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11" t="s">
-        <v>22</v>
+      <c r="A17" s="13"/>
+      <c r="B17" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -748,9 +825,9 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="12" t="s">
-        <v>23</v>
+      <c r="A18" s="14"/>
+      <c r="B18" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -786,7 +863,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15.75">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1"/>
@@ -796,8 +873,8 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="8" t="s">
-        <v>9</v>
+      <c r="A23" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -806,8 +883,8 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="8" t="s">
-        <v>14</v>
+      <c r="A24" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -817,7 +894,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>

</xml_diff>